<commit_message>
hWh: documentor voor respec
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waterschapshuis/props/Waterschapshuis.xlsx
+++ b/src/main/resources/input/Waterschapshuis/props/Waterschapshuis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Waterschapshuis\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302A6FAA-C56D-4ADB-866C-8EC337F2DD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8D2C3-CF1E-41FE-825A-373F375A6A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -976,9 +976,6 @@
     <t>Name of the visuals file</t>
   </si>
   <si>
-    <t>respec</t>
-  </si>
-  <si>
     <t>fullrespec</t>
   </si>
   <si>
@@ -1088,6 +1085,9 @@
   </si>
   <si>
     <t>Vetsion of the extension. When this is a MIM model, specify the MIM extension version</t>
+  </si>
+  <si>
+    <t>documentor</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1563,7 @@
   <dimension ref="A1:U127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
@@ -1663,7 +1663,7 @@
         <v>309</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="2" t="s">
@@ -1679,7 +1679,7 @@
         <v>313</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S2" s="13"/>
       <c r="T2"/>
@@ -2058,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G18" s="14"/>
       <c r="M18" s="14"/>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G21" s="14"/>
       <c r="M21" s="14"/>
@@ -2334,13 +2334,13 @@
     </row>
     <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D27" s="1" t="b">
         <v>0</v>
@@ -2549,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G32" s="14"/>
       <c r="M32" s="14"/>
@@ -2558,13 +2558,13 @@
     </row>
     <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D33" s="1" t="b">
         <v>0</v>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G36" s="14"/>
       <c r="M36" s="14"/>
@@ -2680,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>316</v>
+        <v>353</v>
       </c>
       <c r="G37" s="14"/>
       <c r="M37" s="14"/>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="59" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D59" s="1" t="b">
         <v>0</v>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G73" s="14"/>
       <c r="M73" s="14"/>
@@ -3762,22 +3762,22 @@
     </row>
     <row r="77" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="D77" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="G77" s="14"/>
       <c r="M77" s="14"/>
@@ -3786,22 +3786,22 @@
     </row>
     <row r="78" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>242</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D78" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="D78" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="G78" s="14"/>
       <c r="M78" s="14"/>
@@ -3810,13 +3810,13 @@
     </row>
     <row r="79" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D79" s="1" t="b">
         <v>0</v>
@@ -3826,48 +3826,48 @@
       </c>
       <c r="G79" s="14"/>
       <c r="H79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M79" s="14"/>
       <c r="N79" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S79" s="14"/>
       <c r="T79"/>
     </row>
     <row r="80" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>242</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D80" s="1" t="b">
         <v>0</v>
@@ -3903,13 +3903,13 @@
     </row>
     <row r="82" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D82" s="1" t="b">
         <v>0</v>
@@ -3926,22 +3926,22 @@
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D83" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>335</v>
       </c>
       <c r="G83" s="14"/>
       <c r="M83" s="14"/>
@@ -3949,22 +3949,22 @@
     </row>
     <row r="84" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="D84" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="G84" s="14"/>
       <c r="M84" s="14"/>
@@ -4138,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G91" s="14"/>
       <c r="M91" s="14"/>
@@ -4318,13 +4318,13 @@
     </row>
     <row r="98" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B98" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D98" s="18" t="b">
         <v>0</v>
@@ -4562,7 +4562,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G106" s="14"/>
       <c r="M106" s="14"/>
@@ -5155,7 +5155,7 @@
         <v>0</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G125" s="14"/>
       <c r="M125" s="14"/>

</xml_diff>

<commit_message>
HWH: Updates op properties
Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waterschapshuis/props/Waterschapshuis.xlsx
+++ b/src/main/resources/input/Waterschapshuis/props/Waterschapshuis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Waterschapshuis\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8D2C3-CF1E-41FE-825A-373F375A6A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7CDC9B-4159-4EB1-AA13-A622ABA2FAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="354">
   <si>
     <t>Name</t>
   </si>
@@ -475,9 +475,6 @@
     <t>Language of the metamodel and model. Specify metamodel:model, like "en:nl", or single code for both.</t>
   </si>
   <si>
-    <t>[project-name]-[application-name]-[phase]-[release].office</t>
-  </si>
-  <si>
     <t>refreshxmi</t>
   </si>
   <si>
@@ -1088,6 +1085,9 @@
   </si>
   <si>
     <t>documentor</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -1562,11 +1562,11 @@
   </sheetPr>
   <dimension ref="A1:U127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1604,45 +1604,45 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="G1" s="12"/>
       <c r="H1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M1" s="12"/>
       <c r="N1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S1" s="12"/>
       <c r="T1"/>
@@ -1651,48 +1651,48 @@
       <c r="F2" s="2"/>
       <c r="G2" s="13"/>
       <c r="H2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S2" s="13"/>
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>0</v>
@@ -1755,13 +1755,13 @@
     </row>
     <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="D6" s="5" t="b">
         <v>0</v>
@@ -1807,13 +1807,13 @@
     </row>
     <row r="9" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="D9" s="5" t="b">
         <v>0</v>
@@ -1855,13 +1855,13 @@
     </row>
     <row r="11" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="D11" s="5" t="b">
         <v>0</v>
@@ -1900,22 +1900,22 @@
     </row>
     <row r="13" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="G13" s="14"/>
       <c r="M13" s="14"/>
@@ -1970,10 +1970,10 @@
         <v>19</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>19</v>
@@ -1986,10 +1986,10 @@
         <v>19</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>19</v>
@@ -2023,22 +2023,22 @@
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="G17" s="14"/>
       <c r="M17" s="14"/>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -2058,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G18" s="14"/>
       <c r="M18" s="14"/>
@@ -2067,13 +2067,13 @@
     </row>
     <row r="19" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D19" s="1" t="b">
         <v>0</v>
@@ -2103,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G20" s="14"/>
       <c r="M20" s="14"/>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G21" s="14"/>
       <c r="M21" s="14"/>
@@ -2150,37 +2150,16 @@
       <c r="E22" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F22" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G22" s="14"/>
       <c r="H22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M22" s="14"/>
       <c r="N22" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="S22" s="14"/>
       <c r="T22"/>
@@ -2211,13 +2190,13 @@
     </row>
     <row r="24" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="D24" s="1" t="b">
         <v>0</v>
@@ -2297,100 +2276,58 @@
       <c r="E26" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G26" s="14"/>
       <c r="H26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M26" s="14"/>
       <c r="N26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S26" s="14"/>
       <c r="T26"/>
     </row>
     <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="D27" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M27" s="14"/>
       <c r="N27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S27" s="14"/>
     </row>
     <row r="28" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="D28" s="1" t="b">
         <v>0</v>
@@ -2473,50 +2410,23 @@
       <c r="E30" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F30" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G30" s="14"/>
-      <c r="H30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M30" s="14"/>
-      <c r="N30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S30" s="14"/>
       <c r="T30"/>
     </row>
     <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="D31" s="1" t="b">
         <v>0</v>
@@ -2534,13 +2444,13 @@
     </row>
     <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D32" s="1" t="b">
         <v>0</v>
@@ -2549,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G32" s="14"/>
       <c r="M32" s="14"/>
@@ -2558,14 +2468,14 @@
     </row>
     <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="D33" s="1" t="b">
         <v>0</v>
       </c>
@@ -2576,22 +2486,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="14"/>
-      <c r="I33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M33" s="14"/>
-      <c r="R33" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S33" s="14"/>
     </row>
     <row r="34" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2620,13 +2515,13 @@
     </row>
     <row r="35" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="D35" s="1" t="b">
         <v>0</v>
@@ -2641,14 +2536,14 @@
     </row>
     <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="D36" s="1" t="b">
         <v>0</v>
       </c>
@@ -2656,7 +2551,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G36" s="14"/>
       <c r="M36" s="14"/>
@@ -2665,14 +2560,14 @@
     </row>
     <row r="37" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="D37" s="1" t="b">
         <v>0</v>
       </c>
@@ -2680,7 +2575,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G37" s="14"/>
       <c r="M37" s="14"/>
@@ -2703,51 +2598,24 @@
       <c r="E38" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F38" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G38" s="14"/>
-      <c r="H38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M38" s="14"/>
-      <c r="N38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S38" s="14"/>
       <c r="T38"/>
     </row>
     <row r="39" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>274</v>
-      </c>
       <c r="D39" s="18" t="b">
         <v>0</v>
       </c>
@@ -2758,18 +2626,6 @@
         <v>16</v>
       </c>
       <c r="G39" s="19"/>
-      <c r="I39" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J39" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="K39" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="L39" s="18" t="s">
-        <v>4</v>
-      </c>
       <c r="M39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39"/>
@@ -2790,38 +2646,11 @@
       <c r="E40" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F40" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G40" s="14"/>
-      <c r="H40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M40" s="14"/>
-      <c r="N40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S40" s="14"/>
       <c r="T40"/>
     </row>
@@ -2865,50 +2694,23 @@
       <c r="E42" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F42" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G42" s="14"/>
-      <c r="H42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M42" s="14"/>
-      <c r="N42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S42" s="14"/>
       <c r="T42"/>
     </row>
     <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D43" s="1" t="b">
         <v>0</v>
@@ -2918,48 +2720,48 @@
       </c>
       <c r="G43" s="14"/>
       <c r="H43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M43" s="14"/>
       <c r="N43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="S43" s="14"/>
       <c r="T43"/>
     </row>
     <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="D44" s="1" t="b">
         <v>0</v>
@@ -3016,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G46" s="14"/>
       <c r="M46" s="14"/>
@@ -3059,13 +2861,13 @@
     </row>
     <row r="49" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="D49" s="1" t="b">
         <v>0</v>
@@ -3119,7 +2921,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G51" s="15"/>
       <c r="M51" s="14"/>
@@ -3128,7 +2930,7 @@
     </row>
     <row r="52" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -3145,13 +2947,13 @@
     </row>
     <row r="53" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="D53" s="5" t="b">
         <v>0</v>
@@ -3169,14 +2971,14 @@
     </row>
     <row r="54" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>185</v>
-      </c>
       <c r="D54" s="5" t="b">
         <v>0</v>
       </c>
@@ -3184,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G54" s="14"/>
       <c r="M54" s="14"/>
@@ -3265,13 +3067,13 @@
     </row>
     <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="D58" s="1" t="b">
         <v>0</v>
@@ -3289,14 +3091,14 @@
     </row>
     <row r="59" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D59" s="1" t="b">
         <v>0</v>
       </c>
@@ -3304,45 +3106,21 @@
         <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G59" s="14"/>
-      <c r="I59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M59" s="14"/>
-      <c r="O59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R59" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S59" s="14"/>
     </row>
     <row r="60" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A60" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D60" s="11" t="b">
         <v>0</v>
@@ -3367,22 +3145,22 @@
     </row>
     <row r="61" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="D61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="D61" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="G61" s="14"/>
       <c r="M61" s="14"/>
@@ -3391,13 +3169,13 @@
     </row>
     <row r="62" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D62" s="5" t="b">
         <v>0</v>
@@ -3423,13 +3201,13 @@
     </row>
     <row r="63" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="D63" s="5" t="b">
         <v>0</v>
@@ -3444,13 +3222,13 @@
     </row>
     <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B64" t="s">
         <v>82</v>
       </c>
       <c r="C64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -3459,7 +3237,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G64" s="14"/>
       <c r="M64" s="14"/>
@@ -3468,22 +3246,22 @@
     </row>
     <row r="65" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B65" t="s">
         <v>82</v>
       </c>
       <c r="C65" t="s">
+        <v>296</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
         <v>297</v>
-      </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>298</v>
       </c>
       <c r="G65" s="14"/>
       <c r="M65" s="14"/>
@@ -3492,14 +3270,14 @@
     </row>
     <row r="66" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="C66" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>243</v>
-      </c>
       <c r="D66" s="11" t="b">
         <v>0</v>
       </c>
@@ -3507,7 +3285,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G66" s="16"/>
       <c r="H66" s="11"/>
@@ -3525,13 +3303,13 @@
     </row>
     <row r="67" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="D67" s="5" t="b">
         <v>0</v>
@@ -3564,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G68" s="14"/>
       <c r="M68" s="14"/>
@@ -3573,13 +3351,13 @@
     </row>
     <row r="69" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
+        <v>288</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>289</v>
-      </c>
-      <c r="B69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>290</v>
       </c>
       <c r="D69" s="1" t="b">
         <v>0</v>
@@ -3612,7 +3390,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G70" s="14"/>
       <c r="M70" s="14"/>
@@ -3621,13 +3399,13 @@
     </row>
     <row r="71" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B71" t="s">
         <v>82</v>
       </c>
       <c r="C71" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -3636,7 +3414,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G71" s="14"/>
       <c r="M71" s="14"/>
@@ -3660,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G72" s="14"/>
       <c r="M72" s="14"/>
@@ -3684,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G73" s="14"/>
       <c r="M73" s="14"/>
@@ -3693,14 +3471,14 @@
     </row>
     <row r="74" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="D74" s="1" t="b">
         <v>0</v>
       </c>
@@ -3708,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G74" s="14"/>
       <c r="M74" s="14"/>
@@ -3717,22 +3495,22 @@
     </row>
     <row r="75" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D75" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="G75" s="14"/>
       <c r="M75" s="14"/>
@@ -3762,22 +3540,22 @@
     </row>
     <row r="77" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="D77" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="G77" s="14"/>
       <c r="M77" s="14"/>
@@ -3786,22 +3564,22 @@
     </row>
     <row r="78" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="D78" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="G78" s="14"/>
       <c r="M78" s="14"/>
@@ -3810,13 +3588,13 @@
     </row>
     <row r="79" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D79" s="1" t="b">
         <v>0</v>
@@ -3826,48 +3604,48 @@
       </c>
       <c r="G79" s="14"/>
       <c r="H79" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M79" s="14"/>
       <c r="N79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="S79" s="14"/>
       <c r="T79"/>
     </row>
     <row r="80" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="D80" s="1" t="b">
         <v>0</v>
@@ -3882,13 +3660,13 @@
     </row>
     <row r="81" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D81" s="1" t="b">
         <v>0</v>
@@ -3903,13 +3681,13 @@
     </row>
     <row r="82" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D82" s="1" t="b">
         <v>0</v>
@@ -3918,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G82" s="14"/>
       <c r="M82" s="14"/>
@@ -3926,22 +3704,22 @@
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="D83" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>334</v>
       </c>
       <c r="G83" s="14"/>
       <c r="M83" s="14"/>
@@ -3949,22 +3727,22 @@
     </row>
     <row r="84" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="D84" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="G84" s="14"/>
       <c r="M84" s="14"/>
@@ -3996,13 +3774,13 @@
     </row>
     <row r="86" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="D86" s="1" t="b">
         <v>0</v>
@@ -4030,13 +3808,13 @@
     </row>
     <row r="87" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D87" s="1" t="b">
         <v>1</v>
@@ -4114,7 +3892,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>149</v>
+        <v>353</v>
       </c>
       <c r="G90" s="14"/>
       <c r="M90" s="14"/>
@@ -4138,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G91" s="14"/>
       <c r="M91" s="14"/>
@@ -4147,13 +3925,13 @@
     </row>
     <row r="92" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="D92" s="1" t="b">
         <v>0</v>
@@ -4171,14 +3949,14 @@
     </row>
     <row r="93" spans="1:20" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A93" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B93" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>201</v>
-      </c>
       <c r="D93" s="5" t="b">
         <v>0</v>
       </c>
@@ -4186,7 +3964,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G93" s="14"/>
       <c r="M93" s="14"/>
@@ -4211,35 +3989,35 @@
       </c>
       <c r="G94" s="14"/>
       <c r="H94" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M94" s="14"/>
       <c r="N94" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P94" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R94" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="S94" s="14"/>
       <c r="T94"/>
@@ -4294,13 +4072,13 @@
     </row>
     <row r="97" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A97" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="D97" s="5" t="b">
         <v>0</v>
@@ -4318,13 +4096,13 @@
     </row>
     <row r="98" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="18" t="s">
         <v>320</v>
-      </c>
-      <c r="B98" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="18" t="s">
-        <v>321</v>
       </c>
       <c r="D98" s="18" t="b">
         <v>0</v>
@@ -4380,7 +4158,7 @@
     </row>
     <row r="100" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -4427,13 +4205,13 @@
     </row>
     <row r="101" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="D101" s="1" t="b">
         <v>0</v>
@@ -4466,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G102" s="14"/>
       <c r="M102" s="14"/>
@@ -4475,14 +4253,14 @@
     </row>
     <row r="103" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="D103" s="1" t="b">
         <v>0</v>
       </c>
@@ -4490,7 +4268,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G103" s="14"/>
       <c r="M103" s="14"/>
@@ -4499,22 +4277,22 @@
     </row>
     <row r="104" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="D104" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>251</v>
       </c>
       <c r="G104" s="14"/>
       <c r="M104" s="14"/>
@@ -4523,13 +4301,13 @@
     </row>
     <row r="105" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
       </c>
       <c r="C105" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D105" s="1" t="b">
         <v>1</v>
@@ -4547,13 +4325,13 @@
     </row>
     <row r="106" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B106" t="s">
         <v>10</v>
       </c>
       <c r="C106" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D106" t="b">
         <v>1</v>
@@ -4562,7 +4340,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G106" s="14"/>
       <c r="M106" s="14"/>
@@ -4611,7 +4389,7 @@
         <v>1</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G108" s="14"/>
       <c r="M108" s="14"/>
@@ -4644,13 +4422,13 @@
     </row>
     <row r="110" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="D110" s="1" t="b">
         <v>0</v>
@@ -4725,7 +4503,7 @@
         <v>0</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G113" s="14"/>
       <c r="M113" s="14"/>
@@ -4749,7 +4527,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G114" s="14"/>
       <c r="M114" s="14"/>
@@ -4796,38 +4574,11 @@
       <c r="E116" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F116" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G116" s="14"/>
-      <c r="H116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L116" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M116" s="14"/>
-      <c r="N116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q116" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R116" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S116" s="14"/>
       <c r="T116"/>
     </row>
@@ -4847,38 +4598,11 @@
       <c r="E117" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F117" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G117" s="14"/>
-      <c r="H117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L117" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M117" s="14"/>
-      <c r="N117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R117" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S117" s="14"/>
       <c r="T117"/>
     </row>
@@ -4898,50 +4622,23 @@
       <c r="E118" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F118" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G118" s="14"/>
-      <c r="H118" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L118" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M118" s="14"/>
-      <c r="N118" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R118" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S118" s="14"/>
       <c r="T118"/>
     </row>
     <row r="119" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="D119" s="1" t="b">
         <v>0</v>
@@ -4959,13 +4656,13 @@
     </row>
     <row r="120" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
+        <v>277</v>
+      </c>
+      <c r="B120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" t="s">
         <v>278</v>
-      </c>
-      <c r="B120" t="s">
-        <v>5</v>
-      </c>
-      <c r="C120" t="s">
-        <v>279</v>
       </c>
       <c r="D120" t="b">
         <v>0</v>
@@ -5032,44 +4729,23 @@
       <c r="E122" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F122" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G122" s="14"/>
       <c r="H122" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I122" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J122" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K122" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L122" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M122" s="14"/>
       <c r="N122" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O122" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P122" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q122" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R122" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S122" s="14"/>
       <c r="T122"/>
     </row>
     <row r="123" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>5</v>
@@ -5083,50 +4759,29 @@
       <c r="E123" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F123" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G123" s="14"/>
       <c r="H123" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I123" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J123" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K123" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L123" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M123" s="14"/>
       <c r="N123" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O123" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P123" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q123" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R123" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S123" s="14"/>
       <c r="T123"/>
     </row>
     <row r="124" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D124" s="1" t="b">
         <v>1</v>
@@ -5155,7 +4810,7 @@
         <v>0</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G125" s="14"/>
       <c r="M125" s="14"/>
@@ -5164,22 +4819,22 @@
     </row>
     <row r="126" spans="1:21" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A126" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D126" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E126" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="D126" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E126" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="G126" s="14"/>
       <c r="M126" s="14"/>
@@ -5203,7 +4858,7 @@
         <v>0</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G127" s="14"/>
       <c r="M127" s="14"/>
@@ -5246,48 +4901,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>